<commit_message>
Add test cases for login page and email field 1
</commit_message>
<xml_diff>
--- a/Choice_Stationery_Supplies_Test_cases_Login_Page_and_Email_field.xlsx
+++ b/Choice_Stationery_Supplies_Test_cases_Login_Page_and_Email_field.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <r>
       <rPr>
@@ -217,18 +217,6 @@
 Email:")(%$#@gmail.com</t>
   </si>
   <si>
-    <t>1.Open Browser 
-2.Open URL
-3.Go to the Login page
-4.Enter the maximum allowed length value in the "Email" field.</t>
-  </si>
-  <si>
-    <t>1.The browser is opened
-2.Ecommerce website is opened
-3.The login page is opened
-4.The "Email" field does not allow  to enter a value longer than 128 characters</t>
-  </si>
-  <si>
     <t>TC_log_15</t>
   </si>
   <si>
@@ -488,22 +476,6 @@
 2.Open URL
 3.Go to the Login page
 4.Find the placeholder in the "Email" Field</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Failed. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The placeholder  is not
-present in the "Email" Field </t>
-    </r>
   </si>
   <si>
     <r>
@@ -542,20 +514,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Failed. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The "Email" field can allow  a value 
-longer  than 128 characters.</t>
-    </r>
+    <t>NO RUN</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1135,7 +1094,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>24</v>
@@ -1144,13 +1103,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1161,7 +1120,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>24</v>
@@ -1170,13 +1129,13 @@
         <v>23</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1187,7 +1146,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>24</v>
@@ -1196,10 +1155,10 @@
         <v>23</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>20</v>
@@ -1213,7 +1172,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>24</v>
@@ -1222,10 +1181,10 @@
         <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>20</v>
@@ -1239,7 +1198,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>24</v>
@@ -1248,13 +1207,13 @@
         <v>23</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1265,7 +1224,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>24</v>
@@ -1274,10 +1233,10 @@
         <v>23</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>20</v>
@@ -1317,7 +1276,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>24</v>
@@ -1326,13 +1285,13 @@
         <v>23</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="H18" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1343,7 +1302,7 @@
         <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>24</v>
@@ -1352,10 +1311,10 @@
         <v>23</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>20</v>
@@ -1366,7 +1325,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>39</v>
@@ -1392,7 +1351,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>43</v>
@@ -1404,13 +1363,13 @@
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1418,7 +1377,7 @@
         <v>42</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>45</v>
@@ -1436,33 +1395,25 @@
         <v>46</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
       <c r="H23" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1470,22 +1421,22 @@
         <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>20</v>
@@ -1493,13 +1444,13 @@
     </row>
     <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>24</v>
@@ -1508,10 +1459,10 @@
         <v>23</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>20</v>

</xml_diff>